<commit_message>
updated clean.py with new code and add crimebystates folder
</commit_message>
<xml_diff>
--- a/data no meta/h08_no_meta.xlsx
+++ b/data no meta/h08_no_meta.xlsx
@@ -1,28 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brenden\Desktop\Info Project\hw3\data_no_meta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brenden\PycharmProjects\hwa3_group2\data no meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A606DFDA-0245-4279-A857-308A823FE2B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A27D6B5-48F9-4189-A77F-A8BC7ACD7916}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="h08" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -247,7 +240,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -833,23 +826,23 @@
     <xf numFmtId="0" fontId="1" fillId="35" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="34" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1171,7 +1164,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BS111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1186,225 +1179,225 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="9"/>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="9"/>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="9"/>
-      <c r="AJ1" s="9"/>
-      <c r="AK1" s="9"/>
-      <c r="AL1" s="9"/>
-      <c r="AM1" s="9"/>
-      <c r="AN1" s="9"/>
-      <c r="AO1" s="9"/>
-      <c r="AP1" s="9"/>
-      <c r="AQ1" s="9"/>
-      <c r="AR1" s="9"/>
-      <c r="AS1" s="9"/>
-      <c r="AT1" s="9"/>
-      <c r="AU1" s="9"/>
-      <c r="AV1" s="9"/>
-      <c r="AW1" s="9"/>
-      <c r="AX1" s="9"/>
-      <c r="AY1" s="9"/>
-      <c r="AZ1" s="9"/>
-      <c r="BA1" s="9"/>
-      <c r="BB1" s="9"/>
-      <c r="BC1" s="9"/>
-      <c r="BD1" s="9"/>
-      <c r="BE1" s="9"/>
-      <c r="BF1" s="9"/>
-      <c r="BG1" s="9"/>
-      <c r="BH1" s="9"/>
-      <c r="BI1" s="9"/>
-      <c r="BJ1" s="9"/>
-      <c r="BK1" s="9"/>
-      <c r="BL1" s="9"/>
-      <c r="BM1" s="9"/>
-      <c r="BN1" s="9"/>
-      <c r="BO1" s="9"/>
-      <c r="BP1" s="9"/>
-      <c r="BQ1" s="9"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="7"/>
+      <c r="AH1" s="7"/>
+      <c r="AI1" s="7"/>
+      <c r="AJ1" s="7"/>
+      <c r="AK1" s="7"/>
+      <c r="AL1" s="7"/>
+      <c r="AM1" s="7"/>
+      <c r="AN1" s="7"/>
+      <c r="AO1" s="7"/>
+      <c r="AP1" s="7"/>
+      <c r="AQ1" s="7"/>
+      <c r="AR1" s="7"/>
+      <c r="AS1" s="7"/>
+      <c r="AT1" s="7"/>
+      <c r="AU1" s="7"/>
+      <c r="AV1" s="7"/>
+      <c r="AW1" s="7"/>
+      <c r="AX1" s="7"/>
+      <c r="AY1" s="7"/>
+      <c r="AZ1" s="7"/>
+      <c r="BA1" s="7"/>
+      <c r="BB1" s="7"/>
+      <c r="BC1" s="7"/>
+      <c r="BD1" s="7"/>
+      <c r="BE1" s="7"/>
+      <c r="BF1" s="7"/>
+      <c r="BG1" s="7"/>
+      <c r="BH1" s="7"/>
+      <c r="BI1" s="7"/>
+      <c r="BJ1" s="7"/>
+      <c r="BK1" s="7"/>
+      <c r="BL1" s="7"/>
+      <c r="BM1" s="7"/>
+      <c r="BN1" s="7"/>
+      <c r="BO1" s="7"/>
+      <c r="BP1" s="7"/>
+      <c r="BQ1" s="7"/>
     </row>
     <row r="2" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="8">
         <v>2017</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="8">
+      <c r="C2" s="9"/>
+      <c r="D2" s="10">
         <v>2016</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="8">
+      <c r="E2" s="9"/>
+      <c r="F2" s="10">
         <v>2015</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="8">
+      <c r="G2" s="9"/>
+      <c r="H2" s="10">
         <v>2014</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="9"/>
+      <c r="J2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="8" t="s">
+      <c r="K2" s="9"/>
+      <c r="L2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="11"/>
-      <c r="N2" s="8">
+      <c r="M2" s="9"/>
+      <c r="N2" s="10">
         <v>2012</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="8">
+      <c r="O2" s="9"/>
+      <c r="P2" s="10">
         <v>2011</v>
       </c>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="8" t="s">
+      <c r="Q2" s="9"/>
+      <c r="R2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="11"/>
-      <c r="T2" s="8" t="s">
+      <c r="S2" s="9"/>
+      <c r="T2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="11"/>
-      <c r="V2" s="8">
+      <c r="U2" s="9"/>
+      <c r="V2" s="10">
         <v>2008</v>
       </c>
-      <c r="W2" s="11"/>
-      <c r="X2" s="8">
+      <c r="W2" s="9"/>
+      <c r="X2" s="10">
         <v>2007</v>
       </c>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="8">
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="10">
         <v>2006</v>
       </c>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="8">
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="10">
         <v>2005</v>
       </c>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="8" t="s">
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="8">
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="10">
         <v>2003</v>
       </c>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="8">
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="10">
         <v>2002</v>
       </c>
-      <c r="AI2" s="11"/>
-      <c r="AJ2" s="8">
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="10">
         <v>2001</v>
       </c>
-      <c r="AK2" s="11"/>
-      <c r="AL2" s="8" t="s">
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AM2" s="11"/>
-      <c r="AN2" s="8" t="s">
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AO2" s="11"/>
-      <c r="AP2" s="8">
+      <c r="AO2" s="9"/>
+      <c r="AP2" s="10">
         <v>1998</v>
       </c>
-      <c r="AQ2" s="11"/>
-      <c r="AR2" s="8">
+      <c r="AQ2" s="9"/>
+      <c r="AR2" s="10">
         <v>1997</v>
       </c>
-      <c r="AS2" s="11"/>
-      <c r="AT2" s="8">
+      <c r="AS2" s="9"/>
+      <c r="AT2" s="10">
         <v>1996</v>
       </c>
-      <c r="AU2" s="11"/>
-      <c r="AV2" s="8" t="s">
+      <c r="AU2" s="9"/>
+      <c r="AV2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AW2" s="11"/>
-      <c r="AX2" s="8" t="s">
+      <c r="AW2" s="9"/>
+      <c r="AX2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AY2" s="11"/>
-      <c r="AZ2" s="8" t="s">
+      <c r="AY2" s="9"/>
+      <c r="AZ2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="BA2" s="11"/>
-      <c r="BB2" s="8" t="s">
+      <c r="BA2" s="9"/>
+      <c r="BB2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="BC2" s="11"/>
-      <c r="BD2" s="8">
+      <c r="BC2" s="9"/>
+      <c r="BD2" s="10">
         <v>1991</v>
       </c>
-      <c r="BE2" s="11"/>
-      <c r="BF2" s="8">
+      <c r="BE2" s="9"/>
+      <c r="BF2" s="10">
         <v>1990</v>
       </c>
-      <c r="BG2" s="11"/>
-      <c r="BH2" s="8">
+      <c r="BG2" s="9"/>
+      <c r="BH2" s="10">
         <v>1989</v>
       </c>
-      <c r="BI2" s="11"/>
-      <c r="BJ2" s="8">
+      <c r="BI2" s="9"/>
+      <c r="BJ2" s="10">
         <v>1988</v>
       </c>
-      <c r="BK2" s="11"/>
-      <c r="BL2" s="8" t="s">
+      <c r="BK2" s="9"/>
+      <c r="BL2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="BM2" s="11"/>
-      <c r="BN2" s="8">
+      <c r="BM2" s="9"/>
+      <c r="BN2" s="10">
         <v>1986</v>
       </c>
-      <c r="BO2" s="11"/>
-      <c r="BP2" s="8" t="s">
+      <c r="BO2" s="9"/>
+      <c r="BP2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="BQ2" s="11"/>
-      <c r="BR2" s="8" t="s">
+      <c r="BQ2" s="9"/>
+      <c r="BR2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="BS2" s="11"/>
+      <c r="BS2" s="9"/>
     </row>
     <row r="3" spans="1:71" ht="24" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="6" t="s">
         <v>16</v>
       </c>
@@ -12797,225 +12790,225 @@
       </c>
     </row>
     <row r="56" spans="1:71" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
-      <c r="I56" s="10"/>
-      <c r="J56" s="10"/>
-      <c r="K56" s="10"/>
-      <c r="L56" s="10"/>
-      <c r="M56" s="10"/>
-      <c r="N56" s="10"/>
-      <c r="O56" s="10"/>
-      <c r="P56" s="10"/>
-      <c r="Q56" s="10"/>
-      <c r="R56" s="10"/>
-      <c r="S56" s="10"/>
-      <c r="T56" s="10"/>
-      <c r="U56" s="10"/>
-      <c r="V56" s="10"/>
-      <c r="W56" s="10"/>
-      <c r="X56" s="10"/>
-      <c r="Y56" s="10"/>
-      <c r="Z56" s="10"/>
-      <c r="AA56" s="10"/>
-      <c r="AB56" s="10"/>
-      <c r="AC56" s="10"/>
-      <c r="AD56" s="10"/>
-      <c r="AE56" s="10"/>
-      <c r="AF56" s="10"/>
-      <c r="AG56" s="10"/>
-      <c r="AH56" s="10"/>
-      <c r="AI56" s="10"/>
-      <c r="AJ56" s="10"/>
-      <c r="AK56" s="10"/>
-      <c r="AL56" s="10"/>
-      <c r="AM56" s="10"/>
-      <c r="AN56" s="10"/>
-      <c r="AO56" s="10"/>
-      <c r="AP56" s="10"/>
-      <c r="AQ56" s="10"/>
-      <c r="AR56" s="10"/>
-      <c r="AS56" s="10"/>
-      <c r="AT56" s="10"/>
-      <c r="AU56" s="10"/>
-      <c r="AV56" s="10"/>
-      <c r="AW56" s="10"/>
-      <c r="AX56" s="10"/>
-      <c r="AY56" s="10"/>
-      <c r="AZ56" s="10"/>
-      <c r="BA56" s="10"/>
-      <c r="BB56" s="10"/>
-      <c r="BC56" s="10"/>
-      <c r="BD56" s="10"/>
-      <c r="BE56" s="10"/>
-      <c r="BF56" s="10"/>
-      <c r="BG56" s="10"/>
-      <c r="BH56" s="10"/>
-      <c r="BI56" s="10"/>
-      <c r="BJ56" s="10"/>
-      <c r="BK56" s="10"/>
-      <c r="BL56" s="10"/>
-      <c r="BM56" s="10"/>
-      <c r="BN56" s="10"/>
-      <c r="BO56" s="10"/>
-      <c r="BP56" s="10"/>
-      <c r="BQ56" s="10"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="12"/>
+      <c r="K56" s="12"/>
+      <c r="L56" s="12"/>
+      <c r="M56" s="12"/>
+      <c r="N56" s="12"/>
+      <c r="O56" s="12"/>
+      <c r="P56" s="12"/>
+      <c r="Q56" s="12"/>
+      <c r="R56" s="12"/>
+      <c r="S56" s="12"/>
+      <c r="T56" s="12"/>
+      <c r="U56" s="12"/>
+      <c r="V56" s="12"/>
+      <c r="W56" s="12"/>
+      <c r="X56" s="12"/>
+      <c r="Y56" s="12"/>
+      <c r="Z56" s="12"/>
+      <c r="AA56" s="12"/>
+      <c r="AB56" s="12"/>
+      <c r="AC56" s="12"/>
+      <c r="AD56" s="12"/>
+      <c r="AE56" s="12"/>
+      <c r="AF56" s="12"/>
+      <c r="AG56" s="12"/>
+      <c r="AH56" s="12"/>
+      <c r="AI56" s="12"/>
+      <c r="AJ56" s="12"/>
+      <c r="AK56" s="12"/>
+      <c r="AL56" s="12"/>
+      <c r="AM56" s="12"/>
+      <c r="AN56" s="12"/>
+      <c r="AO56" s="12"/>
+      <c r="AP56" s="12"/>
+      <c r="AQ56" s="12"/>
+      <c r="AR56" s="12"/>
+      <c r="AS56" s="12"/>
+      <c r="AT56" s="12"/>
+      <c r="AU56" s="12"/>
+      <c r="AV56" s="12"/>
+      <c r="AW56" s="12"/>
+      <c r="AX56" s="12"/>
+      <c r="AY56" s="12"/>
+      <c r="AZ56" s="12"/>
+      <c r="BA56" s="12"/>
+      <c r="BB56" s="12"/>
+      <c r="BC56" s="12"/>
+      <c r="BD56" s="12"/>
+      <c r="BE56" s="12"/>
+      <c r="BF56" s="12"/>
+      <c r="BG56" s="12"/>
+      <c r="BH56" s="12"/>
+      <c r="BI56" s="12"/>
+      <c r="BJ56" s="12"/>
+      <c r="BK56" s="12"/>
+      <c r="BL56" s="12"/>
+      <c r="BM56" s="12"/>
+      <c r="BN56" s="12"/>
+      <c r="BO56" s="12"/>
+      <c r="BP56" s="12"/>
+      <c r="BQ56" s="12"/>
     </row>
     <row r="57" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="12">
+      <c r="B57" s="8">
         <v>2017</v>
       </c>
-      <c r="C57" s="11"/>
-      <c r="D57" s="8">
+      <c r="C57" s="9"/>
+      <c r="D57" s="10">
         <v>2016</v>
       </c>
-      <c r="E57" s="11"/>
-      <c r="F57" s="8">
+      <c r="E57" s="9"/>
+      <c r="F57" s="10">
         <v>2015</v>
       </c>
-      <c r="G57" s="11"/>
-      <c r="H57" s="8">
+      <c r="G57" s="9"/>
+      <c r="H57" s="10">
         <v>2014</v>
       </c>
-      <c r="I57" s="11"/>
-      <c r="J57" s="8" t="s">
+      <c r="I57" s="9"/>
+      <c r="J57" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K57" s="11"/>
-      <c r="L57" s="8" t="s">
+      <c r="K57" s="9"/>
+      <c r="L57" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="M57" s="11"/>
-      <c r="N57" s="8">
+      <c r="M57" s="9"/>
+      <c r="N57" s="10">
         <v>2012</v>
       </c>
-      <c r="O57" s="11"/>
-      <c r="P57" s="8">
+      <c r="O57" s="9"/>
+      <c r="P57" s="10">
         <v>2011</v>
       </c>
-      <c r="Q57" s="11"/>
-      <c r="R57" s="8" t="s">
+      <c r="Q57" s="9"/>
+      <c r="R57" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="S57" s="11"/>
-      <c r="T57" s="8" t="s">
+      <c r="S57" s="9"/>
+      <c r="T57" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="U57" s="11"/>
-      <c r="V57" s="8">
+      <c r="U57" s="9"/>
+      <c r="V57" s="10">
         <v>2008</v>
       </c>
-      <c r="W57" s="11"/>
-      <c r="X57" s="8">
+      <c r="W57" s="9"/>
+      <c r="X57" s="10">
         <v>2007</v>
       </c>
-      <c r="Y57" s="11"/>
-      <c r="Z57" s="8">
+      <c r="Y57" s="9"/>
+      <c r="Z57" s="10">
         <v>2006</v>
       </c>
-      <c r="AA57" s="11"/>
-      <c r="AB57" s="8">
+      <c r="AA57" s="9"/>
+      <c r="AB57" s="10">
         <v>2005</v>
       </c>
-      <c r="AC57" s="11"/>
-      <c r="AD57" s="8" t="s">
+      <c r="AC57" s="9"/>
+      <c r="AD57" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="AE57" s="11"/>
-      <c r="AF57" s="8">
+      <c r="AE57" s="9"/>
+      <c r="AF57" s="10">
         <v>2003</v>
       </c>
-      <c r="AG57" s="11"/>
-      <c r="AH57" s="8">
+      <c r="AG57" s="9"/>
+      <c r="AH57" s="10">
         <v>2002</v>
       </c>
-      <c r="AI57" s="11"/>
-      <c r="AJ57" s="8">
+      <c r="AI57" s="9"/>
+      <c r="AJ57" s="10">
         <v>2001</v>
       </c>
-      <c r="AK57" s="11"/>
-      <c r="AL57" s="8" t="s">
+      <c r="AK57" s="9"/>
+      <c r="AL57" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AM57" s="11"/>
-      <c r="AN57" s="8" t="s">
+      <c r="AM57" s="9"/>
+      <c r="AN57" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AO57" s="11"/>
-      <c r="AP57" s="8">
+      <c r="AO57" s="9"/>
+      <c r="AP57" s="10">
         <v>1998</v>
       </c>
-      <c r="AQ57" s="11"/>
-      <c r="AR57" s="8">
+      <c r="AQ57" s="9"/>
+      <c r="AR57" s="10">
         <v>1997</v>
       </c>
-      <c r="AS57" s="11"/>
-      <c r="AT57" s="8">
+      <c r="AS57" s="9"/>
+      <c r="AT57" s="10">
         <v>1996</v>
       </c>
-      <c r="AU57" s="11"/>
-      <c r="AV57" s="8" t="s">
+      <c r="AU57" s="9"/>
+      <c r="AV57" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AW57" s="11"/>
-      <c r="AX57" s="8" t="s">
+      <c r="AW57" s="9"/>
+      <c r="AX57" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AY57" s="11"/>
-      <c r="AZ57" s="8" t="s">
+      <c r="AY57" s="9"/>
+      <c r="AZ57" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="BA57" s="11"/>
-      <c r="BB57" s="8" t="s">
+      <c r="BA57" s="9"/>
+      <c r="BB57" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="BC57" s="11"/>
-      <c r="BD57" s="8">
+      <c r="BC57" s="9"/>
+      <c r="BD57" s="10">
         <v>1991</v>
       </c>
-      <c r="BE57" s="11"/>
-      <c r="BF57" s="8">
+      <c r="BE57" s="9"/>
+      <c r="BF57" s="10">
         <v>1990</v>
       </c>
-      <c r="BG57" s="11"/>
-      <c r="BH57" s="8">
+      <c r="BG57" s="9"/>
+      <c r="BH57" s="10">
         <v>1989</v>
       </c>
-      <c r="BI57" s="11"/>
-      <c r="BJ57" s="8">
+      <c r="BI57" s="9"/>
+      <c r="BJ57" s="10">
         <v>1988</v>
       </c>
-      <c r="BK57" s="11"/>
-      <c r="BL57" s="8" t="s">
+      <c r="BK57" s="9"/>
+      <c r="BL57" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="BM57" s="11"/>
-      <c r="BN57" s="8">
+      <c r="BM57" s="9"/>
+      <c r="BN57" s="10">
         <v>1986</v>
       </c>
-      <c r="BO57" s="11"/>
-      <c r="BP57" s="8" t="s">
+      <c r="BO57" s="9"/>
+      <c r="BP57" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="BQ57" s="11"/>
-      <c r="BR57" s="8" t="s">
+      <c r="BQ57" s="9"/>
+      <c r="BR57" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="BS57" s="11"/>
+      <c r="BS57" s="9"/>
     </row>
     <row r="58" spans="1:71" ht="24" x14ac:dyDescent="0.25">
-      <c r="A58" s="8"/>
+      <c r="A58" s="10"/>
       <c r="B58" s="6" t="s">
         <v>16</v>
       </c>
@@ -24410,6 +24403,64 @@
     <row r="111" spans="1:71" ht="13.15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="74">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A56:BQ56"/>
+    <mergeCell ref="BH57:BI57"/>
+    <mergeCell ref="BJ57:BK57"/>
+    <mergeCell ref="BP57:BQ57"/>
+    <mergeCell ref="BR57:BS57"/>
+    <mergeCell ref="AV57:AW57"/>
+    <mergeCell ref="AX57:AY57"/>
+    <mergeCell ref="AZ57:BA57"/>
+    <mergeCell ref="BB57:BC57"/>
+    <mergeCell ref="BD57:BE57"/>
+    <mergeCell ref="BF57:BG57"/>
+    <mergeCell ref="AP57:AQ57"/>
+    <mergeCell ref="AR57:AS57"/>
+    <mergeCell ref="AT57:AU57"/>
+    <mergeCell ref="BL57:BM57"/>
+    <mergeCell ref="BN57:BO57"/>
+    <mergeCell ref="AF57:AG57"/>
+    <mergeCell ref="AH57:AI57"/>
+    <mergeCell ref="AJ57:AK57"/>
+    <mergeCell ref="AL57:AM57"/>
+    <mergeCell ref="AN57:AO57"/>
+    <mergeCell ref="V57:W57"/>
+    <mergeCell ref="X57:Y57"/>
+    <mergeCell ref="Z57:AA57"/>
+    <mergeCell ref="AB57:AC57"/>
+    <mergeCell ref="AD57:AE57"/>
+    <mergeCell ref="L57:M57"/>
+    <mergeCell ref="N57:O57"/>
+    <mergeCell ref="P57:Q57"/>
+    <mergeCell ref="R57:S57"/>
+    <mergeCell ref="T57:U57"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="A1:BQ1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -24426,64 +24477,6 @@
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="L57:M57"/>
-    <mergeCell ref="N57:O57"/>
-    <mergeCell ref="P57:Q57"/>
-    <mergeCell ref="R57:S57"/>
-    <mergeCell ref="T57:U57"/>
-    <mergeCell ref="V57:W57"/>
-    <mergeCell ref="X57:Y57"/>
-    <mergeCell ref="Z57:AA57"/>
-    <mergeCell ref="AB57:AC57"/>
-    <mergeCell ref="AD57:AE57"/>
-    <mergeCell ref="AF57:AG57"/>
-    <mergeCell ref="AH57:AI57"/>
-    <mergeCell ref="AJ57:AK57"/>
-    <mergeCell ref="AL57:AM57"/>
-    <mergeCell ref="AN57:AO57"/>
-    <mergeCell ref="AP57:AQ57"/>
-    <mergeCell ref="AR57:AS57"/>
-    <mergeCell ref="AT57:AU57"/>
-    <mergeCell ref="BL57:BM57"/>
-    <mergeCell ref="BN57:BO57"/>
-    <mergeCell ref="BP57:BQ57"/>
-    <mergeCell ref="BR57:BS57"/>
-    <mergeCell ref="AV57:AW57"/>
-    <mergeCell ref="AX57:AY57"/>
-    <mergeCell ref="AZ57:BA57"/>
-    <mergeCell ref="BB57:BC57"/>
-    <mergeCell ref="BD57:BE57"/>
-    <mergeCell ref="BF57:BG57"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A56:BQ56"/>
-    <mergeCell ref="BH57:BI57"/>
-    <mergeCell ref="BJ57:BK57"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>